<commit_message>
Excel Numeric Cell Value, And Multiple rows data
</commit_message>
<xml_diff>
--- a/Project171/TestData/InputData.xlsx
+++ b/Project171/TestData/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="7950" windowHeight="3495"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="7950" windowHeight="3495" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="189">
   <si>
     <t>ApplicationURl</t>
   </si>
@@ -48,27 +48,12 @@
     <t>Application_url</t>
   </si>
   <si>
-    <t>Singin_nav_button</t>
-  </si>
-  <si>
-    <t>Email_xpath</t>
-  </si>
-  <si>
     <t>Email_InputData</t>
   </si>
   <si>
-    <t>Next_button</t>
-  </si>
-  <si>
-    <t>Password_xpath</t>
-  </si>
-  <si>
     <t>Pwd_inputData</t>
   </si>
   <si>
-    <t>SingInBtn_xpath</t>
-  </si>
-  <si>
     <t>Login_validData</t>
   </si>
   <si>
@@ -583,6 +568,24 @@
   </si>
   <si>
     <t>NewPwd11</t>
+  </si>
+  <si>
+    <t>Email_location</t>
+  </si>
+  <si>
+    <t>Singin_nav_button_location</t>
+  </si>
+  <si>
+    <t>Next_button_location</t>
+  </si>
+  <si>
+    <t>Password_location</t>
+  </si>
+  <si>
+    <t>SingInBtn_location</t>
+  </si>
+  <si>
+    <t>(//a[@data-task='signin'])[1]</t>
   </si>
 </sst>
 </file>
@@ -986,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1023,7 +1026,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1038,7 +1041,7 @@
         <v>10000.120000000001</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1067,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1092,54 +1095,54 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1163,39 +1166,39 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
@@ -1203,202 +1206,202 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B23" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B26" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1427,308 +1430,308 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
         <v>75</v>
       </c>
-      <c r="C6" t="s">
-        <v>80</v>
-      </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1759,10 +1762,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1773,7 +1776,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1785,7 +1788,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1797,7 +1800,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1809,10 +1812,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1823,211 +1826,211 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="32.25" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="36.75" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.5" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" t="s">
         <v>130</v>
-      </c>
-      <c r="C10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="G10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="10" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D12" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30">
       <c r="A13" s="10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2057,87 +2060,87 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
         <v>164</v>
-      </c>
-      <c r="B2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
         <v>165</v>
-      </c>
-      <c r="B3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
         <v>166</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
         <v>167</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>